<commit_message>
No. 1, 2 solve
</commit_message>
<xml_diff>
--- a/정리.xlsx
+++ b/정리.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>문제</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -136,6 +136,25 @@
   </si>
   <si>
     <t>알고리즘이 이게 맞을까… 너무 오래걸림…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10보다 작은 자연수 중에서 3 또는 5의 배수는 3, 5, 6, 9 이고, 이것을 모두 더하면 23입니다.
+1000보다 작은 자연수 중에서 3 또는 5의 배수를 모두 더하면 얼마일까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000보다 작은수니까 i&lt;=1000 이 아니라 i&lt;1000 이지…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피보나치 수열의 각 항은 바로 앞의 항 두 개를 더한 것이 됩니다. 1과 2로 시작하는 경우 이 수열은 아래와 같습니다.
+1, 2, 3, 5, 8, 13, 21, 34, 55, 89, ...
+짝수이면서 4백만 이하인 모든 항을 더하면 얼마가 됩니까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>While조건의 꺽쇠 방향…</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -232,11 +251,11 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="176" formatCode="#&quot;분&quot;"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -274,8 +293,8 @@
   <tableColumns count="4">
     <tableColumn id="1" name="번호" dataDxfId="3"/>
     <tableColumn id="2" name="문제" dataDxfId="2"/>
-    <tableColumn id="3" name="시간" dataDxfId="0"/>
-    <tableColumn id="4" name="피드백" dataDxfId="1"/>
+    <tableColumn id="3" name="시간" dataDxfId="1"/>
+    <tableColumn id="4" name="피드백" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -570,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -600,13 +619,31 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="7">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -614,7 +651,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="7">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -628,7 +665,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="7">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>15</v>

</xml_diff>